<commit_message>
[RTS DORA Incident Reporting] Translation Notes
Description indicates that the translation is not official
</commit_message>
<xml_diff>
--- a/tools/excel/dora/RTS/RTS-DORA-incident-reporting.xlsx
+++ b/tools/excel/dora/RTS/RTS-DORA-incident-reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\dora\RTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F2F073-885C-48C3-A8A1-62C62F7A4D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB7D85-1571-4B12-835E-C8F2844D1EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10410" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -567,269 +567,270 @@
     <t>description[fr]</t>
   </si>
   <si>
-    <t>L’article 20 de la DORA charge les autorités européennes de surveillance (AES) d’élaborer, par l’intermédiaire du comité mixte et en consultation avec la Banque centrale européenne et l’Agence de l’Union européenne pour la cybersécurité, des projets de normes techniques de réglementation (RTS) établissant le contenu des rapports d’incidents liés aux TIC et la notification des cybermenaces significatives, ainsi que les délais impartis aux EF pour signaler ces incidents aux autorités compétentes.
+    <t>RTS DORA - Rapports d’incidents</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Étant donné que le règlement (UE) 2022/2554 vise à harmoniser et à rationaliser les obligations de déclaration des incidents et à veiller à ce que les autorités compétentes et les autres autorités concernées reçoivent toutes les informations nécessaires sur l’incident majeur afin de prendre des mesures de surveillance et de prévenir les effets de contagion potentiels, les rapports d’incidents majeurs soumis par les entités financières aux autorités compétentes devraient fournir des informations essentielles et exhaustives sur l’incident,  de manière cohérente et normalisée pour toutes les entités financières relevant du champ d’application du règlement (UE) 2022/2554.</t>
+  </si>
+  <si>
+    <t>Afin d’assurer l’harmonisation des obligations de déclaration des incidents majeurs et de maintenir une approche cohérente avec la directive (UE) 2022/2555, les délais de déclaration des incidents majeurs devraient être cohérents pour tous les types d’entités financières. Les délais devraient également être cohérents, dans toute la mesure du possible, et au moins équivalents en effet aux exigences énoncées dans la directive (UE) 2022/2555.</t>
+  </si>
+  <si>
+    <t>Afin de prendre les mesures appropriées, les autorités compétentes doivent recevoir des informations sur l’incident majeur dès les premiers stades après que l’incident a été classé comme majeur. Par conséquent, le délai de soumission de la notification initiale devrait être aussi court que possible après la classification de l’incident, mais aussi offrir une certaine souplesse aux entités financières, en particulier pour les modèles d’affaires de services non urgents, avec un délai plus long après que les entités financières ont pris connaissance de l’incident au cas où les entités financières auraient besoin de plus de temps pour traiter l’incident. Afin d’éviter d’imposer une charge de déclaration excessive à l’entité financière au moment où celle-ci sera chargée de gérer l’incident, le contenu de cette notification initiale devrait être limité aux informations les plus importantes.</t>
+  </si>
+  <si>
+    <t>Étant donné qu’après avoir reçu la notification initiale, les autorités compétentes auront besoin d’informations plus détaillées sur l’incident dans le rapport intermédiaire et de l’ensemble des informations pertinentes dans le rapport final pour évaluer plus avant la situation et évaluer les mesures de surveillance qu’elles pourraient vouloir prendre, les délais de notification devraient être tels que les autorités compétentes puissent recevoir les informations en temps utile,  tout en veillant à ce que les entités financières disposent de suffisamment de temps pour obtenir des informations complètes et exactes.</t>
+  </si>
+  <si>
+    <t>Conformément à l’exigence de proportionnalité énoncée à l’article 20, point a), deuxième alinéa, du règlement (UE) 2022/2554, les délais de déclaration ne devraient pas représenter une charge pour les microentreprises et autres entités financières qui ne sont pas importantes. Par conséquent, les délais de déclaration doivent tenir compte, en particulier, des week-ends et des jours fériés.</t>
+  </si>
+  <si>
+    <t>Étant donné que les cybermenaces importantes doivent être signalées sur une base volontaire, les informations demandées ne devraient pas représenter un fardeau pour les entités financières et devraient être plus limitées que les informations demandées pour les incidents majeurs.</t>
+  </si>
+  <si>
+    <t>Le présent règlement se fonde sur les projets de normes techniques de réglementation soumis à la Commission par les autorités européennes de surveillance.</t>
+  </si>
+  <si>
+    <t>Les autorités européennes de surveillance ont mené des consultations publiques ouvertes sur les projets de normes techniques de réglementation sur lesquels se fonde le présent règlement, analysé les coûts et avantages potentiels qui y sont associés et demandé l’avis de la [...] Groupe des parties intéressées constitué conformément à l’article 37 des règlements (UE) n° 1093/2010, (UE) n° 1094/2010 et (CE) n° 1095/2010 du Parlement européen et du Conseil</t>
+  </si>
+  <si>
+    <t>Dispositions générales</t>
+  </si>
+  <si>
+    <t>Les entités financières fournissent la notification initiale, le rapport intermédiaire ou le rapport final dont le contenu est défini dans le présent règlement, conformément à la description et aux instructions énoncées dans le règlement d’application [insérer la référence une fois publiée au JO].</t>
+  </si>
+  <si>
+    <t>Renseignements généraux à fournir dans la notification initiale, les rapports intermédiaires et finaux d’incident majeur</t>
+  </si>
+  <si>
+    <t>Lors de la soumission de la notification initiale, du rapport intermédiaire et du rapport final, les entités financières fournissent les informations générales suivantes :</t>
+  </si>
+  <si>
+    <t>le type de rapport visé à l’article 19, paragraphe 4, du règlement (UE) 2022/2554 ;</t>
+  </si>
+  <si>
+    <t>le nom, le code LEI de l’entité financière et précisez sous quel type d’entités visé à l’article 2, paragraphe 1, du règlement (UE) 2022/2554 elle est agréée ou enregistrée ;</t>
+  </si>
+  <si>
+    <t>le nom et le code d’identification de l’entité qui soumet la déclaration pour l’entité financière ;</t>
+  </si>
+  <si>
+    <t>les noms et les codes LEI de toutes les entités financières couvertes par le rapport agrégé, le cas échéant.</t>
+  </si>
+  <si>
+    <t>les coordonnées des personnes de contact chargées de communiquer avec l’autorité compétente ;</t>
+  </si>
+  <si>
+    <t>l’identification de l’entreprise mère du groupe, le cas échéant ; et</t>
+  </si>
+  <si>
+    <t>devise de déclaration.</t>
+  </si>
+  <si>
+    <t>Contenu des notifications initiales</t>
+  </si>
+  <si>
+    <t>Les entités financières fournissent au moins les informations suivantes sur l’incident dans la notification initiale :</t>
+  </si>
+  <si>
+    <t>Code de référence de l’incident</t>
+  </si>
+  <si>
+    <t>la date et l’heure de la détection et de la classification de l’incident ;</t>
+  </si>
+  <si>
+    <t>description de l’incident ;</t>
+  </si>
+  <si>
+    <t>les critères de classification à l’origine de la déclaration d’incident tels que définis aux [articles 1er à 8 du règlement délégué [insérer le numéro une fois publié au Journal officiel] ;</t>
+  </si>
+  <si>
+    <t>les États membres touchés par l’incident, le cas échéant ;</t>
+  </si>
+  <si>
+    <t>des informations sur la façon dont l’incident a été découvert ;</t>
+  </si>
+  <si>
+    <t>des informations sur l’origine de l’incident, le cas échéant ;</t>
+  </si>
+  <si>
+    <t>l’indication si un plan de continuité des activités a été activé ;</t>
+  </si>
+  <si>
+    <t>des renseignements sur la reclassification de l’incident de majeur à non majeur, le cas échéant ; et</t>
+  </si>
+  <si>
+    <t>d’autres renseignements, le cas échéant.</t>
+  </si>
+  <si>
+    <t>Contenu des rapports intermédiaires</t>
+  </si>
+  <si>
+    <t>Les entités financières fournissent au moins les informations suivantes sur l’incident dans le rapport intermédiaire :</t>
+  </si>
+  <si>
+    <t>le code de référence de l’incident fourni par l’autorité compétente, le cas échéant ;</t>
+  </si>
+  <si>
+    <t>la date et l’heure de l’incident ;</t>
+  </si>
+  <si>
+    <t>la date et l’heure du rétablissement des activités habituelles, le cas échéant ;</t>
+  </si>
+  <si>
+    <t>des informations sur les critères de classification qui ont déclenché le rapport d’incident ;</t>
+  </si>
+  <si>
+    <t>le type d’incident ;</t>
+  </si>
+  <si>
+    <t>les menaces et les techniques utilisées par l’auteur de menace, le cas échéant ;</t>
+  </si>
+  <si>
+    <t>les secteurs fonctionnels et les processus opérationnels touchés ;</t>
+  </si>
+  <si>
+    <t>les composantes d’infrastructure touchées à l’appui des processus opérationnels ;</t>
+  </si>
+  <si>
+    <t>l’impact sur l’intérêt financier des clients ;</t>
+  </si>
+  <si>
+    <t>des informations sur la déclaration à d’autres autorités ;</t>
+  </si>
+  <si>
+    <t>les mesures temporaires prises ou prévues pour se remettre de l’incident ; et</t>
+  </si>
+  <si>
+    <t>des informations sur les indicateurs de compromission, le cas échéant.</t>
+  </si>
+  <si>
+    <t>Contenu des rapports finaux</t>
+  </si>
+  <si>
+    <t>Les entités financières fournissent les informations suivantes sur l’incident dans le rapport final :</t>
+  </si>
+  <si>
+    <t>des renseignements sur les causes profondes de l’incident ;</t>
+  </si>
+  <si>
+    <t>les dates et les heures auxquelles l’incident a été résolu et la cause profonde traitée ;</t>
+  </si>
+  <si>
+    <t>des informations sur la résolution de l’incident ;</t>
+  </si>
+  <si>
+    <t>les informations pertinentes pour les autorités de résolution, le cas échéant ;</t>
+  </si>
+  <si>
+    <t>des informations sur les coûts et les pertes directs et indirects découlant de l’incident et des informations sur les recouvrements financiers ; et</t>
+  </si>
+  <si>
+    <t>des informations sur les incidents récurrents, le cas échéant.</t>
+  </si>
+  <si>
+    <t>Délais pour la notification initiale, le rapport intermédiaire et les rapports finaux visés à l’article 19, paragraphe 4, du règlement (UE) 2022/2554</t>
+  </si>
+  <si>
+    <t>Les délais pour la présentation de la notification initiale et des rapports intermédiaire et final visés à l’article 19, paragraphe 4, points a) à c), du règlement (UE) 2022/2554 sont les suivants :</t>
+  </si>
+  <si>
+    <t>le rapport initial est soumis le plus tôt possible dans les 4 heures suivant la qualification de l’incident majeur, mais au plus tard dans les 24 heures suivant la date à laquelle l’entité financière a pris connaissance de l’incident ;</t>
+  </si>
+  <si>
+    <t>Un rapport intermédiaire est soumis au plus tard dans les 72 heures suivant la soumission de la notification initiale, même si l’état ou le traitement de l’incident n’a pas changé conformément à l’article 19, paragraphe 4, point b), du règlement (UE) 2022/2554. Les entités financières soumettent sans retard injustifié un rapport intermédiaire actualisé, en tout état de cause, lorsque les activités normales ont été rétablies.</t>
+  </si>
+  <si>
+    <t>Le rapport final est soumis au plus tard un mois après la présentation du dernier rapport intermédiaire mis à jour.</t>
+  </si>
+  <si>
+    <t>Lorsqu’un incident qui n’a pas été classé comme majeur dans les 24 heures est classé comme majeur à un stade ultérieur, l’entité financière soumet la notification initiale dans les quatre heures suivant la classification de l’incident.</t>
+  </si>
+  <si>
+    <t>Lorsque les entités financières ne sont pas en mesure de soumettre la notification initiale, le rapport intermédiaire ou le rapport final dans les délais fixés au paragraphe 1, elles en informent l’autorité compétente dans les meilleurs délais, mais au plus tard dans le délai imparti pour la soumission de la notification ou du rapport, et expliquent les raisons de ce retard.</t>
+  </si>
+  <si>
+    <t>Lorsque le délai de présentation d’une notification initiale, d’un rapport intermédiaire ou d’un rapport final tombe un jour de week-end ou un jour férié dans l’État membre de l’entité financière déclarante, celle-ci peut soumettre la notification initiale, les rapports intermédiaires ou finaux au plus tard à midi le jour ouvrable suivant.</t>
+  </si>
+  <si>
+    <t>Le paragraphe 4 ne s’applique pas à la présentation d’une notification initiale et d’un rapport intermédiaire par les établissements de crédit, les contreparties centrales, les opérateurs de plates-formes de négociation et d’autres entités financières identifiées comme entités essentielles ou importantes en vertu des règles nationales transposant l’article 3 de la directive (UE) 2022/2555, ou les entités financières déclarées comme importantes ou systémiques par l’autorité compétente. Dans ce cas, les entités financières appliquent les délais fixés au paragraphe 1.</t>
+  </si>
+  <si>
+    <t>Contenu de la notification volontaire d’une cybermenace importante</t>
+  </si>
+  <si>
+    <t>Le contenu de la notification relative aux cybermenaces significatives conformément à l’article 19, paragraphe 2, du règlement (UE) 2022/2554 couvre :</t>
+  </si>
+  <si>
+    <t>des informations générales sur l’entité déclarante visées à l’article 4 ;</t>
+  </si>
+  <si>
+    <t>la date et l’heure de la détection de la cybermenace importante et tout autre horodatage pertinent lié à la menace ;</t>
+  </si>
+  <si>
+    <t>la description de la cybermenace importante ;</t>
+  </si>
+  <si>
+    <t>des informations sur l’impact potentiel de la cybermenace sur l’entité financière, ses clients et/ou ses contreparties financières ;</t>
+  </si>
+  <si>
+    <t>les critères de classification qui auraient déclenché un rapport d’incident majeur, si la menace cyber s’était matérialisée ;</t>
+  </si>
+  <si>
+    <t>des renseignements sur l’état de la cybermenace et tout changement dans l’activité de menace ;</t>
+  </si>
+  <si>
+    <t>une description des mesures prises par l’entité financière pour empêcher la matérialisation des cybermenaces importantes, le cas échéant ; et</t>
+  </si>
+  <si>
+    <t>des informations sur la notification de la cybermenace à d’autres entités financières ou autorités ;</t>
+  </si>
+  <si>
+    <t>des informations sur les indicateurs de compromission, le cas échéant ; et</t>
+  </si>
+  <si>
+    <t>d’autres informations pertinentes, le cas échéant.</t>
+  </si>
+  <si>
+    <t>Entrée en vigueur</t>
+  </si>
+  <si>
+    <t>Le présent règlement entre en vigueur le vingtième jour suivant celui de sa publication au Journal officiel de l’Union européenne.</t>
+  </si>
+  <si>
+    <t>node11</t>
+  </si>
+  <si>
+    <t>node13</t>
+  </si>
+  <si>
+    <t>node22</t>
+  </si>
+  <si>
+    <t>node34</t>
+  </si>
+  <si>
+    <t>node48</t>
+  </si>
+  <si>
+    <t>node65</t>
+  </si>
+  <si>
+    <t>node77</t>
+  </si>
+  <si>
+    <t>urn_id</t>
+  </si>
+  <si>
+    <t>[Traduction non officielle]
+L’article 20 de la DORA charge les autorités européennes de surveillance (AES) d’élaborer, par l’intermédiaire du comité mixte et en consultation avec la Banque centrale européenne et l’Agence de l’Union européenne pour la cybersécurité, des projets de normes techniques de réglementation (RTS) établissant le contenu des rapports d’incidents liés aux TIC et la notification des cybermenaces significatives, ainsi que les délais impartis aux EF pour signaler ces incidents aux autorités compétentes.
 Voici le lien du deuxième lot de produits de police en vertu de DORA :
 https://www.eiopa.europa.eu/publications/second-batch-policy-products-under-dora_en
 Voici le lien du document :
 https://www.eiopa.europa.eu/document/download/0dfbccfd-97b2-4076-9644-b5cf4566fc6f_en?filename=JC%202024-33%20-%20Final%20report%20on%20the%20draft%20RTS%20and%20ITS%20on%20incident%20reporting.pdf</t>
-  </si>
-  <si>
-    <t>RTS DORA - Rapports d’incidents</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Étant donné que le règlement (UE) 2022/2554 vise à harmoniser et à rationaliser les obligations de déclaration des incidents et à veiller à ce que les autorités compétentes et les autres autorités concernées reçoivent toutes les informations nécessaires sur l’incident majeur afin de prendre des mesures de surveillance et de prévenir les effets de contagion potentiels, les rapports d’incidents majeurs soumis par les entités financières aux autorités compétentes devraient fournir des informations essentielles et exhaustives sur l’incident,  de manière cohérente et normalisée pour toutes les entités financières relevant du champ d’application du règlement (UE) 2022/2554.</t>
-  </si>
-  <si>
-    <t>Afin d’assurer l’harmonisation des obligations de déclaration des incidents majeurs et de maintenir une approche cohérente avec la directive (UE) 2022/2555, les délais de déclaration des incidents majeurs devraient être cohérents pour tous les types d’entités financières. Les délais devraient également être cohérents, dans toute la mesure du possible, et au moins équivalents en effet aux exigences énoncées dans la directive (UE) 2022/2555.</t>
-  </si>
-  <si>
-    <t>Afin de prendre les mesures appropriées, les autorités compétentes doivent recevoir des informations sur l’incident majeur dès les premiers stades après que l’incident a été classé comme majeur. Par conséquent, le délai de soumission de la notification initiale devrait être aussi court que possible après la classification de l’incident, mais aussi offrir une certaine souplesse aux entités financières, en particulier pour les modèles d’affaires de services non urgents, avec un délai plus long après que les entités financières ont pris connaissance de l’incident au cas où les entités financières auraient besoin de plus de temps pour traiter l’incident. Afin d’éviter d’imposer une charge de déclaration excessive à l’entité financière au moment où celle-ci sera chargée de gérer l’incident, le contenu de cette notification initiale devrait être limité aux informations les plus importantes.</t>
-  </si>
-  <si>
-    <t>Étant donné qu’après avoir reçu la notification initiale, les autorités compétentes auront besoin d’informations plus détaillées sur l’incident dans le rapport intermédiaire et de l’ensemble des informations pertinentes dans le rapport final pour évaluer plus avant la situation et évaluer les mesures de surveillance qu’elles pourraient vouloir prendre, les délais de notification devraient être tels que les autorités compétentes puissent recevoir les informations en temps utile,  tout en veillant à ce que les entités financières disposent de suffisamment de temps pour obtenir des informations complètes et exactes.</t>
-  </si>
-  <si>
-    <t>Conformément à l’exigence de proportionnalité énoncée à l’article 20, point a), deuxième alinéa, du règlement (UE) 2022/2554, les délais de déclaration ne devraient pas représenter une charge pour les microentreprises et autres entités financières qui ne sont pas importantes. Par conséquent, les délais de déclaration doivent tenir compte, en particulier, des week-ends et des jours fériés.</t>
-  </si>
-  <si>
-    <t>Étant donné que les cybermenaces importantes doivent être signalées sur une base volontaire, les informations demandées ne devraient pas représenter un fardeau pour les entités financières et devraient être plus limitées que les informations demandées pour les incidents majeurs.</t>
-  </si>
-  <si>
-    <t>Le présent règlement se fonde sur les projets de normes techniques de réglementation soumis à la Commission par les autorités européennes de surveillance.</t>
-  </si>
-  <si>
-    <t>Les autorités européennes de surveillance ont mené des consultations publiques ouvertes sur les projets de normes techniques de réglementation sur lesquels se fonde le présent règlement, analysé les coûts et avantages potentiels qui y sont associés et demandé l’avis de la [...] Groupe des parties intéressées constitué conformément à l’article 37 des règlements (UE) n° 1093/2010, (UE) n° 1094/2010 et (CE) n° 1095/2010 du Parlement européen et du Conseil</t>
-  </si>
-  <si>
-    <t>Dispositions générales</t>
-  </si>
-  <si>
-    <t>Les entités financières fournissent la notification initiale, le rapport intermédiaire ou le rapport final dont le contenu est défini dans le présent règlement, conformément à la description et aux instructions énoncées dans le règlement d’application [insérer la référence une fois publiée au JO].</t>
-  </si>
-  <si>
-    <t>Renseignements généraux à fournir dans la notification initiale, les rapports intermédiaires et finaux d’incident majeur</t>
-  </si>
-  <si>
-    <t>Lors de la soumission de la notification initiale, du rapport intermédiaire et du rapport final, les entités financières fournissent les informations générales suivantes :</t>
-  </si>
-  <si>
-    <t>le type de rapport visé à l’article 19, paragraphe 4, du règlement (UE) 2022/2554 ;</t>
-  </si>
-  <si>
-    <t>le nom, le code LEI de l’entité financière et précisez sous quel type d’entités visé à l’article 2, paragraphe 1, du règlement (UE) 2022/2554 elle est agréée ou enregistrée ;</t>
-  </si>
-  <si>
-    <t>le nom et le code d’identification de l’entité qui soumet la déclaration pour l’entité financière ;</t>
-  </si>
-  <si>
-    <t>les noms et les codes LEI de toutes les entités financières couvertes par le rapport agrégé, le cas échéant.</t>
-  </si>
-  <si>
-    <t>les coordonnées des personnes de contact chargées de communiquer avec l’autorité compétente ;</t>
-  </si>
-  <si>
-    <t>l’identification de l’entreprise mère du groupe, le cas échéant ; et</t>
-  </si>
-  <si>
-    <t>devise de déclaration.</t>
-  </si>
-  <si>
-    <t>Contenu des notifications initiales</t>
-  </si>
-  <si>
-    <t>Les entités financières fournissent au moins les informations suivantes sur l’incident dans la notification initiale :</t>
-  </si>
-  <si>
-    <t>Code de référence de l’incident</t>
-  </si>
-  <si>
-    <t>la date et l’heure de la détection et de la classification de l’incident ;</t>
-  </si>
-  <si>
-    <t>description de l’incident ;</t>
-  </si>
-  <si>
-    <t>les critères de classification à l’origine de la déclaration d’incident tels que définis aux [articles 1er à 8 du règlement délégué [insérer le numéro une fois publié au Journal officiel] ;</t>
-  </si>
-  <si>
-    <t>les États membres touchés par l’incident, le cas échéant ;</t>
-  </si>
-  <si>
-    <t>des informations sur la façon dont l’incident a été découvert ;</t>
-  </si>
-  <si>
-    <t>des informations sur l’origine de l’incident, le cas échéant ;</t>
-  </si>
-  <si>
-    <t>l’indication si un plan de continuité des activités a été activé ;</t>
-  </si>
-  <si>
-    <t>des renseignements sur la reclassification de l’incident de majeur à non majeur, le cas échéant ; et</t>
-  </si>
-  <si>
-    <t>d’autres renseignements, le cas échéant.</t>
-  </si>
-  <si>
-    <t>Contenu des rapports intermédiaires</t>
-  </si>
-  <si>
-    <t>Les entités financières fournissent au moins les informations suivantes sur l’incident dans le rapport intermédiaire :</t>
-  </si>
-  <si>
-    <t>le code de référence de l’incident fourni par l’autorité compétente, le cas échéant ;</t>
-  </si>
-  <si>
-    <t>la date et l’heure de l’incident ;</t>
-  </si>
-  <si>
-    <t>la date et l’heure du rétablissement des activités habituelles, le cas échéant ;</t>
-  </si>
-  <si>
-    <t>des informations sur les critères de classification qui ont déclenché le rapport d’incident ;</t>
-  </si>
-  <si>
-    <t>le type d’incident ;</t>
-  </si>
-  <si>
-    <t>les menaces et les techniques utilisées par l’auteur de menace, le cas échéant ;</t>
-  </si>
-  <si>
-    <t>les secteurs fonctionnels et les processus opérationnels touchés ;</t>
-  </si>
-  <si>
-    <t>les composantes d’infrastructure touchées à l’appui des processus opérationnels ;</t>
-  </si>
-  <si>
-    <t>l’impact sur l’intérêt financier des clients ;</t>
-  </si>
-  <si>
-    <t>des informations sur la déclaration à d’autres autorités ;</t>
-  </si>
-  <si>
-    <t>les mesures temporaires prises ou prévues pour se remettre de l’incident ; et</t>
-  </si>
-  <si>
-    <t>des informations sur les indicateurs de compromission, le cas échéant.</t>
-  </si>
-  <si>
-    <t>Contenu des rapports finaux</t>
-  </si>
-  <si>
-    <t>Les entités financières fournissent les informations suivantes sur l’incident dans le rapport final :</t>
-  </si>
-  <si>
-    <t>des renseignements sur les causes profondes de l’incident ;</t>
-  </si>
-  <si>
-    <t>les dates et les heures auxquelles l’incident a été résolu et la cause profonde traitée ;</t>
-  </si>
-  <si>
-    <t>des informations sur la résolution de l’incident ;</t>
-  </si>
-  <si>
-    <t>les informations pertinentes pour les autorités de résolution, le cas échéant ;</t>
-  </si>
-  <si>
-    <t>des informations sur les coûts et les pertes directs et indirects découlant de l’incident et des informations sur les recouvrements financiers ; et</t>
-  </si>
-  <si>
-    <t>des informations sur les incidents récurrents, le cas échéant.</t>
-  </si>
-  <si>
-    <t>Délais pour la notification initiale, le rapport intermédiaire et les rapports finaux visés à l’article 19, paragraphe 4, du règlement (UE) 2022/2554</t>
-  </si>
-  <si>
-    <t>Les délais pour la présentation de la notification initiale et des rapports intermédiaire et final visés à l’article 19, paragraphe 4, points a) à c), du règlement (UE) 2022/2554 sont les suivants :</t>
-  </si>
-  <si>
-    <t>le rapport initial est soumis le plus tôt possible dans les 4 heures suivant la qualification de l’incident majeur, mais au plus tard dans les 24 heures suivant la date à laquelle l’entité financière a pris connaissance de l’incident ;</t>
-  </si>
-  <si>
-    <t>Un rapport intermédiaire est soumis au plus tard dans les 72 heures suivant la soumission de la notification initiale, même si l’état ou le traitement de l’incident n’a pas changé conformément à l’article 19, paragraphe 4, point b), du règlement (UE) 2022/2554. Les entités financières soumettent sans retard injustifié un rapport intermédiaire actualisé, en tout état de cause, lorsque les activités normales ont été rétablies.</t>
-  </si>
-  <si>
-    <t>Le rapport final est soumis au plus tard un mois après la présentation du dernier rapport intermédiaire mis à jour.</t>
-  </si>
-  <si>
-    <t>Lorsqu’un incident qui n’a pas été classé comme majeur dans les 24 heures est classé comme majeur à un stade ultérieur, l’entité financière soumet la notification initiale dans les quatre heures suivant la classification de l’incident.</t>
-  </si>
-  <si>
-    <t>Lorsque les entités financières ne sont pas en mesure de soumettre la notification initiale, le rapport intermédiaire ou le rapport final dans les délais fixés au paragraphe 1, elles en informent l’autorité compétente dans les meilleurs délais, mais au plus tard dans le délai imparti pour la soumission de la notification ou du rapport, et expliquent les raisons de ce retard.</t>
-  </si>
-  <si>
-    <t>Lorsque le délai de présentation d’une notification initiale, d’un rapport intermédiaire ou d’un rapport final tombe un jour de week-end ou un jour férié dans l’État membre de l’entité financière déclarante, celle-ci peut soumettre la notification initiale, les rapports intermédiaires ou finaux au plus tard à midi le jour ouvrable suivant.</t>
-  </si>
-  <si>
-    <t>Le paragraphe 4 ne s’applique pas à la présentation d’une notification initiale et d’un rapport intermédiaire par les établissements de crédit, les contreparties centrales, les opérateurs de plates-formes de négociation et d’autres entités financières identifiées comme entités essentielles ou importantes en vertu des règles nationales transposant l’article 3 de la directive (UE) 2022/2555, ou les entités financières déclarées comme importantes ou systémiques par l’autorité compétente. Dans ce cas, les entités financières appliquent les délais fixés au paragraphe 1.</t>
-  </si>
-  <si>
-    <t>Contenu de la notification volontaire d’une cybermenace importante</t>
-  </si>
-  <si>
-    <t>Le contenu de la notification relative aux cybermenaces significatives conformément à l’article 19, paragraphe 2, du règlement (UE) 2022/2554 couvre :</t>
-  </si>
-  <si>
-    <t>des informations générales sur l’entité déclarante visées à l’article 4 ;</t>
-  </si>
-  <si>
-    <t>la date et l’heure de la détection de la cybermenace importante et tout autre horodatage pertinent lié à la menace ;</t>
-  </si>
-  <si>
-    <t>la description de la cybermenace importante ;</t>
-  </si>
-  <si>
-    <t>des informations sur l’impact potentiel de la cybermenace sur l’entité financière, ses clients et/ou ses contreparties financières ;</t>
-  </si>
-  <si>
-    <t>les critères de classification qui auraient déclenché un rapport d’incident majeur, si la menace cyber s’était matérialisée ;</t>
-  </si>
-  <si>
-    <t>des renseignements sur l’état de la cybermenace et tout changement dans l’activité de menace ;</t>
-  </si>
-  <si>
-    <t>une description des mesures prises par l’entité financière pour empêcher la matérialisation des cybermenaces importantes, le cas échéant ; et</t>
-  </si>
-  <si>
-    <t>des informations sur la notification de la cybermenace à d’autres entités financières ou autorités ;</t>
-  </si>
-  <si>
-    <t>des informations sur les indicateurs de compromission, le cas échéant ; et</t>
-  </si>
-  <si>
-    <t>d’autres informations pertinentes, le cas échéant.</t>
-  </si>
-  <si>
-    <t>Entrée en vigueur</t>
-  </si>
-  <si>
-    <t>Le présent règlement entre en vigueur le vingtième jour suivant celui de sa publication au Journal officiel de l’Union européenne.</t>
-  </si>
-  <si>
-    <t>node11</t>
-  </si>
-  <si>
-    <t>node13</t>
-  </si>
-  <si>
-    <t>node22</t>
-  </si>
-  <si>
-    <t>node34</t>
-  </si>
-  <si>
-    <t>node48</t>
-  </si>
-  <si>
-    <t>node65</t>
-  </si>
-  <si>
-    <t>node77</t>
-  </si>
-  <si>
-    <t>urn_id</t>
   </si>
 </sst>
 </file>
@@ -985,6 +986,7 @@
       <font>
         <sz val="12"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -999,8 +1001,51 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1023,6 +1068,108 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1060,152 +1207,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Style de tableau 1" pivot="0" count="0" xr9:uid="{4152591E-1A73-4718-8247-8E569C74F18D}"/>
@@ -1222,16 +1223,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3A5108C-4F0C-4AA7-80D7-8385B3FEDF26}" name="Tableau1" displayName="Tableau1" ref="A1:G78" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3A5108C-4F0C-4AA7-80D7-8385B3FEDF26}" name="Tableau1" displayName="Tableau1" ref="A1:G78" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:G78" xr:uid="{A3A5108C-4F0C-4AA7-80D7-8385B3FEDF26}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DF95C8C7-69FA-4452-8175-17C31010E504}" name="assessable" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{9559EE85-B682-4C35-8883-B5B639A419E0}" name="Depth" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{25564AFE-7417-425E-93AB-E508E734BC54}" name="ref_id" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{03B2D8A4-4609-4E05-BFA7-8801C391873E}" name="urn_id" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{065920AD-C46C-43F8-A094-88D630D762B5}" name="name" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8072A5DC-69CF-45E2-AA86-FFD4CFE10915}" name="description" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{001CF872-CE74-4588-864A-443FC3ADA427}" name="description[fr]" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{DF95C8C7-69FA-4452-8175-17C31010E504}" name="assessable" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{9559EE85-B682-4C35-8883-B5B639A419E0}" name="Depth" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{25564AFE-7417-425E-93AB-E508E734BC54}" name="ref_id" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{03B2D8A4-4609-4E05-BFA7-8801C391873E}" name="urn_id" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{065920AD-C46C-43F8-A094-88D630D762B5}" name="name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8072A5DC-69CF-45E2-AA86-FFD4CFE10915}" name="description" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{001CF872-CE74-4588-864A-443FC3ADA427}" name="description[fr]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1524,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1619,15 +1620,15 @@
         <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>173</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1702,15 +1703,15 @@
         <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>173</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1722,7 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1746,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>9</v>
@@ -1770,7 +1771,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
@@ -1787,7 +1788,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -1804,7 +1805,7 @@
         <v>29</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="156" x14ac:dyDescent="0.3">
@@ -1821,7 +1822,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
@@ -1838,7 +1839,7 @@
         <v>33</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -1855,7 +1856,7 @@
         <v>35</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
@@ -1872,7 +1873,7 @@
         <v>37</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -1889,7 +1890,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
@@ -1906,7 +1907,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1923,7 +1924,7 @@
         <v>43</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1935,14 +1936,14 @@
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -1959,7 +1960,7 @@
         <v>47</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -1969,14 +1970,14 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1995,7 +1996,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2014,7 +2015,7 @@
         <v>52</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2033,7 +2034,7 @@
         <v>54</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2052,7 +2053,7 @@
         <v>56</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2071,7 +2072,7 @@
         <v>58</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2090,7 +2091,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2109,7 +2110,7 @@
         <v>62</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2126,7 +2127,7 @@
         <v>64</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2138,14 +2139,14 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2164,7 +2165,7 @@
         <v>67</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2183,7 +2184,7 @@
         <v>69</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2202,7 +2203,7 @@
         <v>71</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2221,7 +2222,7 @@
         <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2240,7 +2241,7 @@
         <v>75</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2259,7 +2260,7 @@
         <v>77</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2278,7 +2279,7 @@
         <v>79</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2297,7 +2298,7 @@
         <v>81</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2316,7 +2317,7 @@
         <v>83</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2335,7 +2336,7 @@
         <v>85</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2352,7 +2353,7 @@
         <v>87</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2364,14 +2365,14 @@
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6" t="s">
         <v>88</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2390,7 +2391,7 @@
         <v>90</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2409,7 +2410,7 @@
         <v>92</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2428,7 +2429,7 @@
         <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2447,7 +2448,7 @@
         <v>96</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2466,7 +2467,7 @@
         <v>98</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2485,7 +2486,7 @@
         <v>100</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2504,7 +2505,7 @@
         <v>102</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2523,7 +2524,7 @@
         <v>104</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2542,7 +2543,7 @@
         <v>106</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2561,10 +2562,10 @@
         <v>108</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>110</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2599,7 +2600,7 @@
         <v>112</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2616,7 +2617,7 @@
         <v>114</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2628,14 +2629,14 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6" t="s">
         <v>115</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2654,7 +2655,7 @@
         <v>117</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2673,7 +2674,7 @@
         <v>119</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2692,7 +2693,7 @@
         <v>121</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2711,7 +2712,7 @@
         <v>123</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2730,7 +2731,7 @@
         <v>125</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2749,7 +2750,7 @@
         <v>127</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2766,7 +2767,7 @@
         <v>129</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -2785,7 +2786,7 @@
         <v>131</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -2804,7 +2805,7 @@
         <v>133</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2823,7 +2824,7 @@
         <v>135</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2842,7 +2843,7 @@
         <v>137</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -2861,7 +2862,7 @@
         <v>139</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2880,7 +2881,7 @@
         <v>141</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
@@ -2899,7 +2900,7 @@
         <v>143</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
@@ -2918,7 +2919,7 @@
         <v>145</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2935,7 +2936,7 @@
         <v>147</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2947,14 +2948,14 @@
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="6" t="s">
         <v>148</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2973,7 +2974,7 @@
         <v>150</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -2992,7 +2993,7 @@
         <v>152</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -3011,7 +3012,7 @@
         <v>154</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -3030,7 +3031,7 @@
         <v>156</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -3049,7 +3050,7 @@
         <v>158</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -3068,7 +3069,7 @@
         <v>160</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -3087,7 +3088,7 @@
         <v>162</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -3106,7 +3107,7 @@
         <v>164</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -3125,7 +3126,7 @@
         <v>166</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -3144,7 +3145,7 @@
         <v>168</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -3161,7 +3162,7 @@
         <v>170</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -3171,14 +3172,14 @@
       </c>
       <c r="C78" s="10"/>
       <c r="D78" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6" t="s">
         <v>171</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>